<commit_message>
Update Zeit + Statusprotokoll
</commit_message>
<xml_diff>
--- a/Protokolle/Statusprotokoll_Arbeitszeitverwaltung_Sprint_1.xlsx
+++ b/Protokolle/Statusprotokoll_Arbeitszeitverwaltung_Sprint_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\GitHub\Arbeitszeitverwaltung_Sport_Camp_Salcher\Protokolle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\GitHub\Arbeitszeitverwaltung_Sportcamp_Salcher\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9373E554-F50C-4FE5-AFDF-337135E2E021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D611064-36D7-4D9C-89BD-4863A38B23ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D76CD718-F911-4B74-8B36-452779118D5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D76CD718-F911-4B74-8B36-452779118D5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
   <si>
     <t>23.9.2019-27.09.2019</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Statusprotokoll, Erstellung der Datenbankanbindung (Umstieg auf Promises), Zeitplan</t>
+  </si>
+  <si>
+    <t>Recherche bzgl. Frontend JavaScript SinglePageArchitecture</t>
+  </si>
+  <si>
+    <t>Tests mit SinglePageArchitecture und Implementierung einer groben Struktur</t>
+  </si>
+  <si>
+    <t>Ausbau Frontend für CRUD Operations</t>
+  </si>
+  <si>
+    <t>Fehlerbehebung bei Ungleichheiten in der Datenbankstruktur und im Frontend</t>
   </si>
 </sst>
 </file>
@@ -567,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629CB0FE-3767-48C8-99DB-4A99BF8A238C}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +703,9 @@
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -723,7 +737,9 @@
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -755,7 +771,9 @@
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -787,7 +805,9 @@
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -819,7 +839,9 @@
       <c r="B29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -851,7 +873,9 @@
       <c r="B33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>